<commit_message>
Update de excel file y se agrego un branch para el campo invalido.
</commit_message>
<xml_diff>
--- a/Data/PruebasCurps.xlsx
+++ b/Data/PruebasCurps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows10\Documents\UiPath\Proyectos\CurpVerification\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E3E580-2207-4C55-B274-50FD10743D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75850C85-4E40-481A-A287-4F8D2CA30DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26810,7 +26810,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -96579,7 +96579,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>